<commit_message>
combined into one file
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_test.xlsx
+++ b/tests/frameworks/framework_test.xlsx
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>Code Name</t>
   </si>
@@ -498,18 +498,6 @@
     <t>Compartment 3</t>
   </si>
   <si>
-    <t>comp_4</t>
-  </si>
-  <si>
-    <t>Compartment 4</t>
-  </si>
-  <si>
-    <t>comp_5</t>
-  </si>
-  <si>
-    <t>Compartment 5</t>
-  </si>
-  <si>
     <t>Components</t>
   </si>
   <si>
@@ -649,36 +637,6 @@
   </si>
   <si>
     <t>Parameter 9</t>
-  </si>
-  <si>
-    <t>par_10</t>
-  </si>
-  <si>
-    <t>Parameter 10</t>
-  </si>
-  <si>
-    <t>par_11</t>
-  </si>
-  <si>
-    <t>Parameter 11</t>
-  </si>
-  <si>
-    <t>par_12</t>
-  </si>
-  <si>
-    <t>Parameter 12</t>
-  </si>
-  <si>
-    <t>par_13</t>
-  </si>
-  <si>
-    <t>Parameter 13</t>
-  </si>
-  <si>
-    <t>par_14</t>
-  </si>
-  <si>
-    <t>Parameter 14</t>
   </si>
   <si>
     <t>Attribute Code Name</t>
@@ -1079,7 +1037,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1177,42 +1135,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="18">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"n,y"</formula1>
     </dataValidation>
@@ -1249,24 +1173,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1275,13 +1181,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="B1" s="2" t="str">
         <f>'Compartments'!A2</f>
         <v>comp_0</v>
@@ -1298,49 +1204,29 @@
         <f>'Compartments'!A5</f>
         <v>comp_3</v>
       </c>
-      <c r="F1" s="2" t="str">
-        <f>'Compartments'!A6</f>
-        <v>comp_4</v>
-      </c>
-      <c r="G1" s="2" t="str">
-        <f>'Compartments'!A7</f>
-        <v>comp_5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="str">
         <f>'Compartments'!A2</f>
         <v>comp_0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="str">
         <f>'Compartments'!A3</f>
         <v>comp_1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="str">
         <f>'Compartments'!A4</f>
         <v>comp_2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="str">
         <f>'Compartments'!A5</f>
         <v>comp_3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="str">
-        <f>'Compartments'!A6</f>
-        <v>comp_4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="str">
-        <f>'Compartments'!A7</f>
-        <v>comp_5</v>
       </c>
     </row>
   </sheetData>
@@ -1373,27 +1259,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>'Compartments'!A2</f>
@@ -1409,10 +1295,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>CONCATENATE('Compartments'!A3,",",A2)</f>
@@ -1431,10 +1317,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>CONCATENATE('Compartments'!A4,",",A3)</f>
@@ -1453,10 +1339,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>CONCATENATE('Compartments'!A5,",",A4)</f>
@@ -1475,19 +1361,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="str">
-        <f>CONCATENATE('Compartments'!A6,",",A5)</f>
-        <v>comp_4,charac_3</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>'Compartments'!A6</f>
-        <v>comp_4</v>
-      </c>
+        <f>A5</f>
+        <v>charac_3</v>
+      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="3" t="str">
         <f>A5</f>
         <v>charac_3</v>
@@ -1497,19 +1380,16 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f>CONCATENATE('Compartments'!A7,",",A6)</f>
-        <v>comp_5,charac_4</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f>'Compartments'!A7</f>
-        <v>comp_5</v>
-      </c>
+        <f>A6</f>
+        <v>charac_4</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3" t="str">
         <f>A6</f>
         <v>charac_4</v>
@@ -1519,10 +1399,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>A7</f>
@@ -1538,10 +1418,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>A8</f>
@@ -1557,10 +1437,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>A9</f>
@@ -1576,10 +1456,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>A10</f>
@@ -1601,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1622,21 +1502,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1644,10 +1524,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1655,10 +1535,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1666,10 +1546,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1677,10 +1557,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1688,10 +1568,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1699,10 +1579,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1710,10 +1590,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1721,10 +1601,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1732,69 +1612,14 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1824,18 +1649,18 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>CONCATENATE(A2,"_att_0")</f>
@@ -1868,10 +1693,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>CONCATENATE(A5,"_att_0")</f>
@@ -1904,10 +1729,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>CONCATENATE(A8,"_att_0")</f>
@@ -1940,10 +1765,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>CONCATENATE(A11,"_att_0")</f>
@@ -1976,10 +1801,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C14" s="3" t="str">
         <f>CONCATENATE(A14,"_att_0")</f>
@@ -2012,10 +1837,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>CONCATENATE(A17,"_att_0")</f>
@@ -2048,10 +1873,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C20" s="3" t="str">
         <f>CONCATENATE(A20,"_att_0")</f>

</xml_diff>